<commit_message>
add function to save in file data
</commit_message>
<xml_diff>
--- a/Poradnik.xlsx
+++ b/Poradnik.xlsx
@@ -595,10 +595,10 @@
     <t xml:space="preserve">ssh-add     skopiować to terminala sciezke prywatna ssh </t>
   </si>
   <si>
-    <t>ssh-add  /c/Users/lenovo/Desktop/BURY_PRACA/Projekty/GitHub/C/ssh_github</t>
-  </si>
-  <si>
     <t>git clone git@github.com:piotrek291c/C.git</t>
+  </si>
+  <si>
+    <t>ssh-add  /c/Users/lenovo/Desktop/BURY_PRACA/Projekty/GitHub/ssh_github</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -886,7 +886,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1164,7 +1164,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1175,7 +1175,7 @@
   <dimension ref="A1:H247"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+      <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1836,12 +1836,12 @@
     </row>
     <row r="143" spans="1:1" s="6" customFormat="1">
       <c r="A143" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:1" s="6" customFormat="1">
       <c r="A144" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="145" s="6" customFormat="1"/>

</xml_diff>

<commit_message>
add argument in function
</commit_message>
<xml_diff>
--- a/Poradnik.xlsx
+++ b/Poradnik.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="195">
   <si>
     <t>Service Name</t>
   </si>
@@ -599,6 +599,15 @@
   </si>
   <si>
     <t>ssh-add  /c/Users/lenovo/Desktop/BURY_PRACA/Projekty/GitHub/ssh_github</t>
+  </si>
+  <si>
+    <t>open the file C:\Program Files\Git\etc\ssh\ssh_config</t>
+  </si>
+  <si>
+    <t>Simply add a new line and save it:</t>
+  </si>
+  <si>
+    <t>IdentityFile "C:/Users/lenovo/Desktop/BURY_PRACA/Projekty/GitHub/ssh_github"</t>
   </si>
 </sst>
 </file>
@@ -842,7 +851,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -886,7 +895,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1164,7 +1173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1175,7 +1184,7 @@
   <dimension ref="A1:H247"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1844,22 +1853,34 @@
         <v>190</v>
       </c>
     </row>
-    <row r="145" s="6" customFormat="1"/>
-    <row r="146" s="6" customFormat="1"/>
-    <row r="147" s="6" customFormat="1"/>
-    <row r="148" s="6" customFormat="1"/>
-    <row r="149" s="6" customFormat="1"/>
-    <row r="150" s="6" customFormat="1"/>
-    <row r="151" s="6" customFormat="1"/>
-    <row r="152" s="6" customFormat="1"/>
-    <row r="153" s="6" customFormat="1"/>
-    <row r="154" s="6" customFormat="1"/>
-    <row r="155" s="6" customFormat="1"/>
-    <row r="156" s="6" customFormat="1"/>
-    <row r="157" s="6" customFormat="1"/>
-    <row r="158" s="6" customFormat="1"/>
-    <row r="159" s="6" customFormat="1"/>
-    <row r="160" s="6" customFormat="1"/>
+    <row r="145" spans="1:1" s="6" customFormat="1"/>
+    <row r="146" spans="1:1" s="6" customFormat="1">
+      <c r="A146" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" s="6" customFormat="1">
+      <c r="A147" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" s="6" customFormat="1">
+      <c r="A148" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" s="6" customFormat="1"/>
+    <row r="150" spans="1:1" s="6" customFormat="1"/>
+    <row r="151" spans="1:1" s="6" customFormat="1"/>
+    <row r="152" spans="1:1" s="6" customFormat="1"/>
+    <row r="153" spans="1:1" s="6" customFormat="1"/>
+    <row r="154" spans="1:1" s="6" customFormat="1"/>
+    <row r="155" spans="1:1" s="6" customFormat="1"/>
+    <row r="156" spans="1:1" s="6" customFormat="1"/>
+    <row r="157" spans="1:1" s="6" customFormat="1"/>
+    <row r="158" spans="1:1" s="6" customFormat="1"/>
+    <row r="159" spans="1:1" s="6" customFormat="1"/>
+    <row r="160" spans="1:1" s="6" customFormat="1"/>
     <row r="161" spans="1:1" s="6" customFormat="1"/>
     <row r="162" spans="1:1" s="6" customFormat="1"/>
     <row r="163" spans="1:1" s="6" customFormat="1"/>

</xml_diff>